<commit_message>
Data base testing done
</commit_message>
<xml_diff>
--- a/ExcelData/TC_ChangeMembership.xlsx
+++ b/ExcelData/TC_ChangeMembership.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="23505" windowHeight="10740"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:V33"/>
+  <oleSize ref="A1:X33"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>categoryName</t>
   </si>
@@ -40,34 +40,23 @@
     <t>Custom Date</t>
   </si>
   <si>
-    <t>15 September 2023</t>
-  </si>
-  <si>
-    <t>30 September 2023</t>
-  </si>
-  <si>
-    <t>Mosco Package 03</t>
-  </si>
-  <si>
-    <t>Mosco_Unlimited</t>
+    <t>Westwood Packages One Time</t>
+  </si>
+  <si>
+    <t>8 September 2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF17171B"/>
-      <name val="Inter"/>
     </font>
     <font>
       <sz val="14"/>
@@ -80,11 +69,6 @@
       <color rgb="FF2A00FF"/>
       <name val="Courier New"/>
       <family val="3"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFF4594E"/>
-      <name val="Inter"/>
     </font>
     <font>
       <sz val="12"/>
@@ -112,20 +96,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,16 +388,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -435,30 +417,16 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="18.75">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="18.75">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>